<commit_message>
- edit some column excel
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Report/BaoCaoChietKhau/Teamplate_BaoCaoTongHopHoaHongNhanVien.xlsx
+++ b/banhang24/Template/ExportExcel/Report/BaoCaoChietKhau/Teamplate_BaoCaoTongHopHoaHongNhanVien.xlsx
@@ -19,122 +19,31 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>Tổng cộng:</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Mã nhân viên
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(1)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Tên nhân viên
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(2)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Hoa hồng thực hiện
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(3)</t>
-    </r>
-  </si>
-  <si>
     <t>BÁO CÁO TỔNG HỢP HOA HỒNG THEO NHÂN VIÊN</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Hoa hồng thực hiện theo Y/cầu
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(4)</t>
-    </r>
+    <t>Mã nhân viên</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Hoa hồng tư vấn
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(5)</t>
-    </r>
+    <t>Tên nhân viên</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Hoa hồng bán gói dịch vụ
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(6)</t>
-    </r>
+    <t>Hoa hồng thực hiện</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Tổng
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(7= 3+4+5 + 6)</t>
-    </r>
+    <t>Hoa hồng tư vấn</t>
+  </si>
+  <si>
+    <t>Hoa hồng bán gói dịch vụ</t>
+  </si>
+  <si>
+    <t>Tổng</t>
+  </si>
+  <si>
+    <t>Tổng cộng</t>
+  </si>
+  <si>
+    <t>Hoa hồng NV hỗ trợ</t>
   </si>
 </sst>
 </file>
@@ -210,7 +119,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -225,19 +134,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -262,7 +158,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -319,9 +215,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -636,7 +529,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,7 +546,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -664,13 +557,13 @@
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
     </row>
     <row r="3" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15"/>
@@ -695,16 +588,16 @@
         <v>3</v>
       </c>
       <c r="D5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="G5" s="9" t="s">
         <v>6</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -925,9 +818,9 @@
     </row>
     <row r="30" spans="1:7" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B30" s="22"/>
+        <v>7</v>
+      </c>
+      <c r="B30" s="21"/>
       <c r="C30" s="10">
         <f>SUM(C$6:C29)</f>
         <v>0</v>

</xml_diff>